<commit_message>
structural development for characters and decks
</commit_message>
<xml_diff>
--- a/Documentation/Daily planning.xlsx
+++ b/Documentation/Daily planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s133911\Desktop\CardAdventureGame\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BA6DE59-4AE9-49F3-A473-442A77865F0E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97775C98-BE7C-400A-A2F5-735B4C54279E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9A258FC2-4D7D-4798-95F7-1A7FD96CACD9}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>Detailed planning, defining scope</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>Drag and Drop for cards, hand layout</t>
+  </si>
+  <si>
+    <t>More structure changes</t>
+  </si>
+  <si>
+    <t>Created Decks and methods for decks. Also structure for Characters</t>
   </si>
 </sst>
 </file>
@@ -511,7 +517,7 @@
   <dimension ref="A2:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,7 +604,9 @@
       <c r="C8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="7" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -610,7 +618,9 @@
       <c r="C9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">

</xml_diff>